<commit_message>
Se agrega restricción de zonas Norte, Centro y Sur
</commit_message>
<xml_diff>
--- a/datos_salida/Distribución_Combustibles_Unidades.xlsx
+++ b/datos_salida/Distribución_Combustibles_Unidades.xlsx
@@ -3284,21 +3284,21 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>Ninguno</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>Ninguno</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>G90</t>
+          <t>Ninguno</t>
         </is>
       </c>
       <c r="J68" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -3326,21 +3326,21 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>Ninguno</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>Ninguno</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>G90</t>
+          <t>Ninguno</t>
         </is>
       </c>
       <c r="J69" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -4754,21 +4754,21 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>Ninguno</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Ninguno</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>Ninguno</t>
+          <t>G90</t>
         </is>
       </c>
       <c r="J103" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="104">

</xml_diff>